<commit_message>
Big Robot for order + Update of Fork
</commit_message>
<xml_diff>
--- a/MECHANICAL/STRUCTURE/SMALL_ROBOT/SmallRobotPerimeter.xlsx
+++ b/MECHANICAL/STRUCTURE/SMALL_ROBOT/SmallRobotPerimeter.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\git\cen-meca\MECHANICAL\STRUCTURE\SMALL_ROBOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A53175-2DCA-4D97-AFB8-FA8B68C11A9F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22CF1EA-C681-43E8-A9B1-FC778CB41E9E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{E7B70F99-CB0D-4E6D-AC58-C2169FD3B9ED}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{E7B70F99-CB0D-4E6D-AC58-C2169FD3B9ED}"/>
   </bookViews>
   <sheets>
     <sheet name="SmallRobotPerimeter" sheetId="1" r:id="rId1"/>
+    <sheet name="BigRobotPerimeter" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>Bottom Cut</t>
   </si>
@@ -384,8 +385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C5E1FD-C8CB-458E-8A8D-892A813E3FBE}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,4 +460,65 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A966E355-4168-4132-B06A-3AC204364149}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>A4</f>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f>A3</f>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>SUM(A2:A7)</f>
+        <v>934</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>